<commit_message>
aggiunto il keep negli indici
</commit_message>
<xml_diff>
--- a/SWC.xlsx
+++ b/SWC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marco.pluchino\Desktop\Marco\finance\2021_FinanceJupyterTutorial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65994A7F-86FF-4964-97C3-9BB1137DD601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A2A2B1-3EC7-46F5-9E1C-3A0311AA5CFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="history" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="71">
   <si>
     <t>VALUE</t>
   </si>
@@ -250,6 +250,9 @@
   </si>
   <si>
     <t>strategy</t>
+  </si>
+  <si>
+    <t>https://medium.com/analytics-vidhya/how-to-create-a-python-library-7d5aea80cc3f</t>
   </si>
 </sst>
 </file>
@@ -1002,9 +1005,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A2CEF33-8E12-4CDA-B380-6F256EC5837A}">
   <dimension ref="A5:F10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1076,14 +1079,20 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C10" s="1"/>
+      <c r="B10" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1" xr:uid="{C90A1460-4E86-4FE3-B162-2D78E211E438}"/>
+    <hyperlink ref="B10" r:id="rId2" xr:uid="{BA6309F6-83A7-4276-8B67-93B5F1B38B87}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1272,8 +1281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3825EC27-4DDD-40C3-BCDE-475F29058754}">
   <dimension ref="A2:N17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>